<commit_message>
update for the crdc
</commit_message>
<xml_diff>
--- a/cds_configuration_files/cds-synthetic_data_values.xlsx
+++ b/cds_configuration_files/cds-synthetic_data_values.xlsx
@@ -14,15 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>phs_accession</t>
   </si>
   <si>
-    <t/>
+    <t>phs0001</t>
   </si>
   <si>
-    <t>phs0001</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -84,14 +84,14 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -425,317 +425,315 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="3"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="2"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="2"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="2"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="2"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="2"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="2"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="2"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="2"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="2"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="2"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
-      <c r="A14" s="3"/>
+      <c r="A14" s="2"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="3"/>
+      <c r="A15" s="2"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="2"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="2"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="2"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="2"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="2"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="2"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
-      <c r="A22" s="3"/>
+      <c r="A22" s="2"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>